<commit_message>
added the date format checks to the application
</commit_message>
<xml_diff>
--- a/TestData/qcTest.xlsx
+++ b/TestData/qcTest.xlsx
@@ -79,7 +79,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -110,6 +110,12 @@
         <bgColor rgb="FFFFADB0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFC5"/>
+        <bgColor rgb="FFFFFFC5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -123,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -267,6 +273,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="170" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8904,87 +8929,93 @@
       </c>
     </row>
     <row r="99" ht="45" customHeight="1" s="17">
-      <c r="A99" s="12" t="inlineStr">
+      <c r="A99" s="73" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B99" s="13" t="n">
+      <c r="B99" s="74" t="n">
         <v>13233</v>
       </c>
-      <c r="C99" s="12" t="n"/>
-      <c r="D99" s="12" t="n"/>
-      <c r="E99" s="12" t="n"/>
-      <c r="F99" s="12" t="inlineStr">
+      <c r="C99" s="73" t="n"/>
+      <c r="D99" s="73" t="n"/>
+      <c r="E99" s="73" t="n"/>
+      <c r="F99" s="73" t="inlineStr">
         <is>
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="H99" s="12" t="inlineStr">
+      <c r="G99" s="75" t="n"/>
+      <c r="H99" s="73" t="inlineStr">
         <is>
           <t>Index to S.K.C. Bulletins 101-147, typed photocopy</t>
         </is>
       </c>
-      <c r="I99" s="12" t="inlineStr">
+      <c r="I99" s="73" t="inlineStr">
         <is>
           <t>Stanley-G.I. Electric Manufacturing Company</t>
         </is>
       </c>
-      <c r="J99" s="12" t="n"/>
-      <c r="K99" s="12" t="n"/>
-      <c r="L99" s="12" t="n"/>
-      <c r="M99" s="12" t="n"/>
-      <c r="N99" s="12" t="inlineStr">
+      <c r="J99" s="73" t="n"/>
+      <c r="K99" s="73" t="n"/>
+      <c r="L99" s="73" t="n"/>
+      <c r="M99" s="73" t="n"/>
+      <c r="N99" s="73" t="inlineStr">
         <is>
           <t>Stanley Electric Manufacturing Company (Pittsfield, Mass.)</t>
         </is>
       </c>
-      <c r="O99" s="12" t="n"/>
-      <c r="P99" s="13" t="inlineStr">
+      <c r="O99" s="73" t="n"/>
+      <c r="P99" s="74" t="inlineStr">
         <is>
           <t>Unknown</t>
         </is>
       </c>
-      <c r="Q99" s="12" t="n"/>
-      <c r="R99" s="12" t="inlineStr">
+      <c r="Q99" s="73" t="n"/>
+      <c r="R99" s="73" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S99" s="12" t="inlineStr">
+      <c r="S99" s="73" t="inlineStr">
         <is>
           <t>2 pages</t>
         </is>
       </c>
-      <c r="T99" s="18" t="n"/>
-      <c r="U99" s="18" t="inlineStr">
+      <c r="T99" s="76" t="n"/>
+      <c r="U99" s="76" t="inlineStr">
         <is>
           <t>Scan each bulletin as it's own file, glass down</t>
         </is>
       </c>
-      <c r="V99" s="12" t="inlineStr">
+      <c r="V99" s="73" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B03.F08.Bull.Index101.147</t>
         </is>
       </c>
-      <c r="W99" s="20" t="n">
+      <c r="W99" s="77" t="n">
         <v>45432</v>
       </c>
-      <c r="X99" s="12" t="inlineStr">
+      <c r="X99" s="73" t="inlineStr">
         <is>
           <t>LW</t>
         </is>
       </c>
-      <c r="Y99" s="19" t="inlineStr">
+      <c r="Y99" s="78" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z99" s="19" t="inlineStr">
+      <c r="Z99" s="78" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
+      <c r="AA99" s="75" t="n"/>
+      <c r="AB99" s="75" t="n"/>
+      <c r="AC99" s="75" t="n"/>
+      <c r="AD99" s="75" t="n"/>
+      <c r="AE99" s="75" t="n"/>
     </row>
     <row r="100" ht="45" customHeight="1" s="17">
       <c r="A100" s="12" t="inlineStr">
@@ -42618,84 +42649,89 @@
       <c r="AD104" s="6" t="n"/>
     </row>
     <row r="105" ht="15" customHeight="1" s="17">
-      <c r="A105" s="15" t="inlineStr">
+      <c r="A105" s="79" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B105" s="2" t="n">
+      <c r="B105" s="80" t="n">
         <v>13275</v>
       </c>
-      <c r="C105" s="16" t="n"/>
-      <c r="D105" s="16" t="n"/>
-      <c r="E105" s="16" t="n"/>
-      <c r="F105" s="15" t="inlineStr">
+      <c r="C105" s="81" t="n"/>
+      <c r="D105" s="81" t="n"/>
+      <c r="E105" s="81" t="n"/>
+      <c r="F105" s="79" t="inlineStr">
         <is>
           <t>"Apparatus for Transmission of Light and Power"</t>
         </is>
       </c>
-      <c r="G105" s="16" t="n"/>
-      <c r="H105" s="15" t="inlineStr">
+      <c r="G105" s="81" t="n"/>
+      <c r="H105" s="79" t="inlineStr">
         <is>
           <t>Apparatus for Transmission of Light and Power</t>
         </is>
       </c>
-      <c r="I105" s="15" t="inlineStr">
+      <c r="I105" s="79" t="inlineStr">
         <is>
           <t xml:space="preserve">"C.C Chesney" transcribed on front cover. </t>
         </is>
       </c>
-      <c r="J105" s="15" t="inlineStr">
+      <c r="J105" s="79" t="inlineStr">
         <is>
           <t>The Royal Electric Co. (Montreal, Canada)</t>
         </is>
       </c>
-      <c r="K105" s="16" t="n"/>
-      <c r="L105" s="16" t="n"/>
-      <c r="M105" s="2" t="n">
+      <c r="K105" s="81" t="n"/>
+      <c r="L105" s="81" t="n"/>
+      <c r="M105" s="80" t="n">
         <v>1896</v>
       </c>
-      <c r="N105" s="16" t="n"/>
-      <c r="O105" s="16" t="n"/>
-      <c r="P105" s="16" t="n"/>
-      <c r="Q105" s="15" t="inlineStr">
+      <c r="N105" s="81" t="n"/>
+      <c r="O105" s="81" t="n"/>
+      <c r="P105" s="81" t="n"/>
+      <c r="Q105" s="79" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="R105" s="16" t="n"/>
-      <c r="S105" s="15" t="inlineStr">
+      <c r="R105" s="81" t="n"/>
+      <c r="S105" s="79" t="inlineStr">
         <is>
           <t>Copyright Undetermind</t>
         </is>
       </c>
-      <c r="T105" s="16" t="n"/>
-      <c r="U105" s="16" t="inlineStr">
+      <c r="T105" s="81" t="n"/>
+      <c r="U105" s="81" t="inlineStr">
         <is>
           <t>Box 6, Folder 4, Item 2</t>
         </is>
       </c>
-      <c r="V105" s="16" t="inlineStr">
+      <c r="V105" s="81" t="inlineStr">
         <is>
           <t>Glass Down. Do not scan duplicate. Scan copy with C.C Chesney written on front</t>
         </is>
       </c>
-      <c r="W105" s="15" t="inlineStr">
+      <c r="W105" s="79" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B06.F04.02</t>
         </is>
       </c>
-      <c r="X105" s="30" t="n">
+      <c r="X105" s="82" t="n">
         <v>45496</v>
       </c>
-      <c r="Y105" s="16" t="inlineStr">
+      <c r="Y105" s="81" t="inlineStr">
         <is>
           <t>MC,GH</t>
         </is>
       </c>
-      <c r="Z105" s="16" t="n"/>
-      <c r="AB105" s="19" t="n"/>
-      <c r="AD105" s="6" t="n"/>
+      <c r="Z105" s="81" t="n"/>
+      <c r="AA105" s="75" t="n"/>
+      <c r="AB105" s="78" t="n"/>
+      <c r="AC105" s="75" t="n"/>
+      <c r="AD105" s="83" t="n"/>
+      <c r="AE105" s="75" t="n"/>
+      <c r="AF105" s="75" t="n"/>
+      <c r="AG105" s="75" t="n"/>
     </row>
     <row r="106" ht="165" customHeight="1" s="17">
       <c r="A106" s="15" t="inlineStr">

</xml_diff>